<commit_message>
updated apis and script
</commit_message>
<xml_diff>
--- a/dataset/chittor_ipos.xlsx
+++ b/dataset/chittor_ipos.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="chittor_ipos.csv" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="ipos.csv" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11924,9 +11924,6 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="2" max="2" width="42.0"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">

</xml_diff>